<commit_message>
Fixed some double white spaces in IT
</commit_message>
<xml_diff>
--- a/tools/excel/iso27001/iso27001-2022.xlsx
+++ b/tools/excel/iso27001/iso27001-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgorlani/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59909A5D-B93C-3843-99FC-8AC5D9ED29EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405CC4EF-7919-6547-BEBE-7A9A63C5FE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47540" yWindow="4780" windowWidth="35840" windowHeight="20400" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47540" yWindow="4780" windowWidth="35840" windowHeight="20400" tabRatio="797" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -4897,324 +4897,51 @@
     <t>Description[it]</t>
   </si>
   <si>
-    <t>Politiche per la sicurezza  delle informazioni</t>
-  </si>
-  <si>
-    <t>La politica di sicurezza delle informazioni e le politiche  specifiche per argomento devono essere definite,  approvate dalla direzione, pubblicate, comunicate e  riconosciute dal personale rilevante e dalle parti  interessate pertinenti, e revisionate a intervalli  pianificati e in caso di cambiamenti significativi.</t>
-  </si>
-  <si>
-    <t>Ruoli e responsabilità per la  sicurezza delle informazioni</t>
-  </si>
-  <si>
-    <t>I ruoli e le responsabilità per la sicurezza delle  informazioni devono essere definiti e assegnati in base  alle esigenze dell'organizzazione.</t>
-  </si>
-  <si>
     <t>Separazione dei compiti</t>
   </si>
   <si>
-    <t>I compiti in conflitto e le aree di responsabilità in  conflitto devono essere separate.</t>
-  </si>
-  <si>
-    <t>Responsabilità della  direzione</t>
-  </si>
-  <si>
-    <t>La direzione deve richiedere a tutto il personale di  applicare la sicurezza delle informazioni in conformità  con la politica di sicurezza delle informazioni stabilita, le  politiche specifiche per argomento e le procedure  dell'organizzazione.</t>
-  </si>
-  <si>
     <t>Contatti con le autorità</t>
   </si>
   <si>
-    <t>L'organizzazione deve stabilire e mantenere contatti  con le autorità pertinenti.</t>
-  </si>
-  <si>
-    <t>Contatti con gruppi di  interesse speciale</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve stabilire e mantenere contatti  con gruppi di interesse speciale o altri forum  specialistici sulla sicurezza e associazioni professionali.</t>
-  </si>
-  <si>
     <t>Intelligence sulle minacce</t>
   </si>
   <si>
-    <t>Le informazioni relative alle minacce alla sicurezza delle  informazioni devono essere raccolte e analizzate per  produrre intelligence sulle minacce.</t>
-  </si>
-  <si>
-    <t>Sicurezza delle informazioni  nella gestione dei progetti</t>
-  </si>
-  <si>
-    <t>La sicurezza delle informazioni deve essere integrata  nella gestione dei progetti.</t>
-  </si>
-  <si>
-    <t>Inventario delle informazioni  e di altri asset associati</t>
-  </si>
-  <si>
-    <t>Deve essere sviluppato e mantenuto un inventario delle  informazioni e degli altri asset associati, inclusi i  proprietari.</t>
-  </si>
-  <si>
-    <t>Utilizzo accettabile delle  informazioni e di altri asset  associati</t>
-  </si>
-  <si>
-    <t>Devono essere identificate, documentate e  implementate regole per l'utilizzo accettabile e  procedure per la gestione delle informazioni e degli altri  asset associati.</t>
-  </si>
-  <si>
     <t>Restituzione degli asset</t>
   </si>
   <si>
-    <t>Il personale e altre parti interessate, se appropriato,  devono restituire tutti gli asset dell'organizzazione in  loro possesso al momento del cambiamento o della  cessazione del loro impiego, contratto o accordo.</t>
-  </si>
-  <si>
-    <t>Classificazione delle  informazioni</t>
-  </si>
-  <si>
-    <t>Le informazioni devono essere classificate in base alle  esigenze di sicurezza delle informazioni  dell'organizzazione, in base a confidenzialità, integrità,  disponibilità e requisiti pertinenti delle parti interessate.</t>
-  </si>
-  <si>
-    <t>Etichettatura delle  informazioni</t>
-  </si>
-  <si>
-    <t>Deve essere sviluppato e implementato un insieme  appropriato di procedure per l'etichettatura delle  informazioni, in conformità con lo schema di  classificazione delle informazioni adottato  dall'organizzazione.</t>
-  </si>
-  <si>
-    <t>Trasferimento delle  informazioni</t>
-  </si>
-  <si>
-    <t>Devono essere in vigore un insieme di regole,  procedure o accordi per il trasferimento delle  informazioni in tutti i tipi di strutture di trasferimento  all'interno dell'organizzazione e tra l'organizzazione e  altre parti.</t>
-  </si>
-  <si>
     <t>Controllo degli accessi</t>
   </si>
   <si>
-    <t>Devono essere stabilite e implementate regole per  controllare l'accesso fisico e logico alle informazioni e  ad altri asset associati, in base ai requisiti aziendali e di  sicurezza delle informazioni.</t>
-  </si>
-  <si>
     <t>Gestione delle identità</t>
   </si>
   <si>
-    <t>Il ciclo di vita completo delle identità deve essere  gestito.</t>
-  </si>
-  <si>
-    <t>Informazioni di  autenticazione</t>
-  </si>
-  <si>
-    <t>L'assegnazione e la gestione delle informazioni di  autenticazione devono essere controllate da un  processo gestionale, incluso l'avviso al personale  sull'adeguato trattamento delle informazioni di  autenticazione.</t>
-  </si>
-  <si>
     <t>Diritti di accesso</t>
   </si>
   <si>
-    <t>I diritti di accesso alle informazioni e ad altri asset  associati devono essere forniti, revisionati, modificati e  rimossi in conformità con la politica specifica per  argomento e le regole dell'organizzazione per il  controllo degli accessi.</t>
-  </si>
-  <si>
-    <t>Sicurezza delle informazioni  nelle relazioni con i fornitori</t>
-  </si>
-  <si>
-    <t>Devono essere definite e implementate procedure e  processi per gestire i rischi per la sicurezza delle  informazioni associati all'uso dei prodotti o servizi del  fornitore.</t>
-  </si>
-  <si>
-    <t>Affrontare la sicurezza delle  informazioni nei contratti  con i fornitori</t>
-  </si>
-  <si>
-    <t>Requisiti pertinenti per la sicurezza delle informazioni  devono essere stabiliti e concordati con ciascun  fornitore in base al tipo di relazione con il fornitore.</t>
-  </si>
-  <si>
-    <t>Gestione della sicurezza  delle informazioni nella  catena di  approvvigionamento ICT</t>
-  </si>
-  <si>
-    <t>Devono essere definiti e implementati processi e  procedure per gestire i rischi per la sicurezza delle  informazioni associati alla catena di  approvvigionamento di prodotti e servizi ICT.</t>
-  </si>
-  <si>
-    <t>Monitoraggio, revisione e  gestione dei servizi dei  fornitori</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve monitorare regolarmente,  revisionare, valutare e gestire i cambiamenti nelle  pratiche di sicurezza delle informazioni e nella fornitura  dei servizi da parte dei fornitori.</t>
-  </si>
-  <si>
-    <t>Sicurezza delle informazioni  per l'uso dei servizi cloud</t>
-  </si>
-  <si>
-    <t>Devono essere stabiliti processi per l'acquisizione, l'uso,  la gestione e l'uscita dai servizi cloud in conformità con i  requisiti di sicurezza delle informazioni  dell'organizzazione.</t>
-  </si>
-  <si>
-    <t>Pianificazione e  preparazione per la gestione  degli incidenti di sicurezza  delle informazioni</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve pianificare e prepararsi per  gestire gli incidenti di sicurezza delle informazioni  definendo, istituendo e comunicando processi, ruoli e  responsabilità per la gestione degli incidenti di  sicurezza delle informazioni.</t>
-  </si>
-  <si>
-    <t>Valutazione e decisione sugli  eventi di sicurezza delle  informazioni</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve valutare gli eventi di sicurezza  delle informazioni e decidere se devono essere  categorizzati come incidenti di sicurezza delle  informazioni.</t>
-  </si>
-  <si>
-    <t>Risposta agli incidenti di  sicurezza delle informazioni</t>
-  </si>
-  <si>
-    <t>Gli incidenti di sicurezza delle informazioni devono  essere gestiti in conformità con le procedure  documentate.</t>
-  </si>
-  <si>
-    <t>Apprendimento dagli  incidenti di sicurezza delle  informazioni</t>
-  </si>
-  <si>
-    <t>Le conoscenze acquisite dagli incidenti di sicurezza delle  informazioni devono essere utilizzate per rafforzare e  migliorare i controlli della sicurezza delle informazioni.</t>
-  </si>
-  <si>
     <t>Raccolta di prove</t>
   </si>
   <si>
-    <t>L'organizzazione deve stabilire e implementare  procedure per l'identificazione, la raccolta,  l'acquisizione e la conservazione di prove relative agli  eventi di sicurezza delle informazioni.</t>
-  </si>
-  <si>
-    <t>Sicurezza delle informazioni  durante la distruzione</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve pianificare come mantenere la  sicurezza delle informazioni ad un livello appropriato  durante la distruzione.</t>
-  </si>
-  <si>
-    <t>Prontezza ICT per la  continuità aziendale</t>
-  </si>
-  <si>
-    <t>La prontezza ICT deve essere pianificata, implementata,  mantenuta e testata in base agli obiettivi di continuità  aziendale e ai requisiti di continuità ICT.</t>
-  </si>
-  <si>
-    <t>Requisiti legali, statutari,  regolamentari e contrattuali</t>
-  </si>
-  <si>
-    <t>I requisiti legali, statutari, regolamentari e contrattuali  rilevanti per la sicurezza delle informazioni devono  essere identificati, documentati e mantenuti aggiornati.</t>
-  </si>
-  <si>
-    <t>Diritti di proprietà  intellettuale</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve implementare procedure  appropriate per proteggere i diritti di proprietà  intellettuale.</t>
-  </si>
-  <si>
     <t>Protezione dei documenti</t>
   </si>
   <si>
-    <t>I documenti devono essere protetti da perdita,  distruzione, falsificazione, accesso non autorizzato e  divulgazione non autorizzata.</t>
-  </si>
-  <si>
-    <t>Privacy e protezione delle  informazioni personali  identificabili (PII)</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve identificare e soddisfare i  requisiti relativi alla tutela della privacy e alla protezione  delle PII in conformità alle leggi, ai regolamenti  applicabili e ai requisiti contrattuali.</t>
-  </si>
-  <si>
-    <t>Revisione indipendente della  sicurezza delle informazioni</t>
-  </si>
-  <si>
-    <t>L'approccio dell'organizzazione alla gestione della  sicurezza delle informazioni e la sua implementazione,  compresi persone, processi e tecnologie, devono essere  periodicamente riesaminati in modo indipendente a  intervalli pianificati o in caso di cambiamenti  significativi.</t>
-  </si>
-  <si>
-    <t>Conformità alle politiche,  regole e standard per la  sicurezza delle informazioni</t>
-  </si>
-  <si>
-    <t>La conformità alla politica di sicurezza delle  informazioni dell'organizzazione, alle politiche  specifiche per argomento, alle regole e agli standard  deve essere regolarmente riesaminata.</t>
-  </si>
-  <si>
-    <t>Procedure operative  documentate</t>
-  </si>
-  <si>
-    <t>Le procedure operative per le strutture di elaborazione  delle informazioni devono essere documentate e messe  a disposizione del personale che ne ha bisogno.</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
-    <t>Verifiche di verifica del background su tutti i candidati  per diventare personale devono essere effettuate  prima di entrare a far parte dell'organizzazione e in  modo continuativo, prendendo in considerazione le  leggi, i regolamenti, l'etica applicabile e  proporzionalmente alle esigenze aziendali, alla  classificazione delle informazioni da accedere e ai rischi  percepiti.</t>
-  </si>
-  <si>
-    <t>Termini e condizioni di  impiego</t>
-  </si>
-  <si>
-    <t>I contratti di lavoro devono specificare le responsabilità  del personale e dell'organizzazione per la sicurezza  delle informazioni.</t>
-  </si>
-  <si>
-    <t>Consapevolezza, formazione  ed educazione sulla  sicurezza delle informazioni</t>
-  </si>
-  <si>
-    <t>Il personale dell'organizzazione e le parti interessate  pertinenti devono ricevere adeguate consapevolezza,  formazione ed educazione sulla sicurezza delle  informazioni e aggiornamenti regolari della politica di  sicurezza delle informazioni dell'organizzazione, delle  politiche specifiche per argomento e delle procedure, in  relazione alle loro mansioni.</t>
-  </si>
-  <si>
     <t>Processo disciplinare</t>
   </si>
   <si>
-    <t>Un processo disciplinare deve essere formalizzato e  comunicato per intraprendere azioni contro il  personale e altre parti interessate pertinenti che hanno  commesso una violazione della politica di sicurezza  delle informazioni.</t>
-  </si>
-  <si>
-    <t>Responsabilità dopo la  cessazione o il cambio di  impiego</t>
-  </si>
-  <si>
-    <t>Le responsabilità e i doveri relativi alla sicurezza delle  informazioni che rimangono validi dopo la cessazione o  il cambio di impiego devono essere definiti, attuati e  comunicati al personale e alle altre parti interessate  pertinenti.</t>
-  </si>
-  <si>
-    <t>Accordi di riservatezza o non  divulgazione</t>
-  </si>
-  <si>
-    <t>Gli accordi di riservatezza o non divulgazione che  riflettono le esigenze dell'organizzazione per la  protezione delle informazioni devono essere  identificati, documentati, regolarmente riesaminati e  firmati dal personale e dalle altre parti interessate  pertinenti.</t>
-  </si>
-  <si>
     <t>Lavoro remoto</t>
   </si>
   <si>
-    <t>Devono essere implementate misure di sicurezza  quando il personale lavora in remoto per proteggere le  informazioni a cui si accede, elabora o memorizza al di  fuori dei locali dell'organizzazione.</t>
-  </si>
-  <si>
-    <t>Segnalazione degli eventi  relativi alla sicurezza delle  informazioni</t>
-  </si>
-  <si>
-    <t>L'organizzazione deve fornire un meccanismo affinché  il personale possa segnalare in modo tempestivo eventi  di sicurezza delle informazioni osservati o sospettati  attraverso canali appropriati.</t>
-  </si>
-  <si>
     <t>Perimetri di sicurezza fisica</t>
   </si>
   <si>
-    <t>I perimetri di sicurezza devono essere definiti e  utilizzati per proteggere aree che contengono  informazioni e altri asset associati.</t>
-  </si>
-  <si>
     <t>Accesso fisico</t>
   </si>
   <si>
-    <t>Le aree sicure devono essere protette da controlli di  accesso appropriati e punti di accesso.</t>
-  </si>
-  <si>
-    <t>Sicurezza degli uffici, delle  stanze e delle strutture</t>
-  </si>
-  <si>
-    <t>La sicurezza fisica degli uffici, delle stanze e delle  strutture deve essere progettata e implementata.</t>
-  </si>
-  <si>
-    <t>Monitoraggio della sicurezza  fisica</t>
-  </si>
-  <si>
-    <t>I locali devono essere monitorati continuamente per  l'accesso fisico non autorizzato.</t>
-  </si>
-  <si>
-    <t>Protezione contro minacce  fisiche e ambientali</t>
-  </si>
-  <si>
-    <t>La protezione contro minacce fisiche ed ambientali,  come disastri naturali o altre minacce fisiche  intenzionali o non intenzionali all'infrastruttura, deve  essere progettata ed implementata.</t>
-  </si>
-  <si>
     <t>Lavoro in aree sicure</t>
   </si>
   <si>
-    <t>Misure di sicurezza per lavorare in aree sicure devono  essere progettate ed implementate.</t>
-  </si>
-  <si>
-    <t>Area di lavoro e schermo  puliti</t>
-  </si>
-  <si>
-    <t>Norme per la pulizia della scrivania per documenti e  supporti rimovibili e regole per lo schermo dei sistemi  di elaborazione delle informazioni devono essere  definite e applicate in modo appropriato.</t>
-  </si>
-  <si>
-    <t>Posizionamento e  protezione dell'attrezzatura</t>
-  </si>
-  <si>
-    <t>L'attrezzatura deve essere posizionata in modo sicuro e  protetta.</t>
-  </si>
-  <si>
     <t>Sicurezza dei beni fuori sede</t>
   </si>
   <si>
@@ -5224,237 +4951,63 @@
     <t>Supporti di memorizzazione</t>
   </si>
   <si>
-    <t>I supporti di memorizzazione devono essere gestiti  durante il loro ciclo di vita di acquisizione, utilizzo,  trasporto e smaltimento in conformità con lo schema di  classificazione e i requisiti di gestione  dell'organizzazione.</t>
-  </si>
-  <si>
     <t>Servizi di supporto</t>
   </si>
   <si>
-    <t>Le strutture di elaborazione delle informazioni devono  essere protette da interruzioni di corrente e da altre  interruzioni causate da malfunzionamenti nei servizi di  supporto.</t>
-  </si>
-  <si>
     <t>Sicurezza dei cavi</t>
   </si>
   <si>
-    <t>I cavi che trasportano alimentazione, dati o servizi di  informazione di supporto devono essere protetti da  intercettazioni, interferenze o danneggiamenti.</t>
-  </si>
-  <si>
-    <t>Manutenzione  dell'attrezzatura</t>
-  </si>
-  <si>
-    <t>L'attrezzatura deve essere mantenuta correttamente  per garantire la disponibilità, l'integrità e la riservatezza  delle informazioni.</t>
-  </si>
-  <si>
-    <t>Smaltimento sicuro o  riutilizzo dell'attrezzatura</t>
-  </si>
-  <si>
-    <t>Gli elementi di attrezzatura contenenti supporti di  memorizzazione devono essere verificati per garantire  che tutti i dati sensibili e i software con licenza siano  stati rimossi o sovrascritti in modo sicuro prima dello  smaltimento o riutilizzo.</t>
-  </si>
-  <si>
-    <t>Dispositivi terminali  dell'utente</t>
-  </si>
-  <si>
-    <t>Le informazioni memorizzate su, elaborate da o  accessibili tramite dispositivi terminali dell'utente  devono essere protette.</t>
-  </si>
-  <si>
     <t>Diritti di accesso privilegiati</t>
   </si>
   <si>
-    <t>L'assegnazione e l'uso dei diritti di accesso privilegiati  devono essere limitati e gestiti.</t>
-  </si>
-  <si>
-    <t>Restrizione dell'accesso alle  informazioni</t>
-  </si>
-  <si>
-    <t>L'accesso alle informazioni e ad altri asset associati  deve essere limitato in conformità con la politica  specifica per argomento sul controllo degli accessi.</t>
-  </si>
-  <si>
     <t>Accesso al codice sorgente</t>
   </si>
   <si>
-    <t>L'accesso in lettura e scrittura al codice sorgente, agli  strumenti di sviluppo e alle librerie software deve  essere gestito in modo appropriato.</t>
-  </si>
-  <si>
     <t>Autenticazione sicura</t>
   </si>
   <si>
-    <t>Tecnologie e procedure di autenticazione sicura devono  essere implementate in base alle restrizioni di accesso  alle informazioni e alla politica specifica per argomento  sul controllo degli accessi.</t>
-  </si>
-  <si>
     <t>Gestione delle capacità</t>
   </si>
   <si>
-    <t>L'uso delle risorse deve essere monitorato e adattato in  linea con i requisiti di capacità attuali e previsti.</t>
-  </si>
-  <si>
     <t>Protezione contro malware</t>
   </si>
   <si>
-    <t>La protezione contro malware deve essere  implementata e supportata da un'adeguata  consapevolezza degli utenti.</t>
-  </si>
-  <si>
-    <t>Gestione delle vulnerabilità  tecniche</t>
-  </si>
-  <si>
-    <t>Deve essere ottenuta informazione sulle vulnerabilità  tecniche dei sistemi informativi in uso, valutata  l'esposizione dell'organizzazione a tali vulnerabilità e  adottate misure appropriate.</t>
-  </si>
-  <si>
-    <t>Gestione della  configurazione</t>
-  </si>
-  <si>
-    <t>Le configurazioni, inclusa la configurazione della  sicurezza, dell'hardware, del software, dei servizi e delle  reti, devono essere stabilite, documentate,  implementate, monitorate e revisionate.</t>
-  </si>
-  <si>
-    <t>Eliminazione delle  informazioni</t>
-  </si>
-  <si>
-    <t>Le informazioni memorizzate nei sistemi informativi,  nei dispositivi o in qualsiasi altro supporto di  memorizzazione devono essere eliminate quando non  sono più necessarie.</t>
-  </si>
-  <si>
     <t>Mascheramento dei dati</t>
   </si>
   <si>
-    <t>Il mascheramento dei dati deve essere utilizzato in  conformità con la politica specifica per argomento  sull'accesso e altre politiche specifiche correlate, e ai  requisiti aziendali, considerando la legislazione  applicabile.</t>
-  </si>
-  <si>
-    <t>Prevenzione della fuga di  dati</t>
-  </si>
-  <si>
-    <t>Misure di prevenzione della fuga di dati devono essere  applicate a sistemi, reti e ad altri dispositivi che  elaborano, memorizzano o trasmettono informazioni  sensibili.</t>
-  </si>
-  <si>
     <t>Backup delle informazioni</t>
   </si>
   <si>
-    <t>Copie di backup di informazioni, software e sistemi  devono essere mantenute e regolarmente testate in  conformità con la politica specifica per argomento sul  backup concordata.</t>
-  </si>
-  <si>
-    <t>Ridondanza delle strutture  di elaborazione delle  informazioni</t>
-  </si>
-  <si>
-    <t>Le strutture di elaborazione delle informazioni devono  essere implementate con una ridondanza sufficiente  per soddisfare i requisiti di disponibilità.</t>
-  </si>
-  <si>
     <t>Registrazione</t>
   </si>
   <si>
-    <t>I registri che registrano attività, eccezioni, guasti e altri  eventi rilevanti devono essere prodotti, memorizzati,  protetti ed analizzati.</t>
-  </si>
-  <si>
     <t>Monitoraggio delle attività</t>
   </si>
   <si>
-    <t>Reti, sistemi e applicazioni devono essere monitorati  per comportamenti anomali e devono essere adottate  azioni appropriate per valutare potenziali incidenti di  sicurezza delle informazioni.</t>
-  </si>
-  <si>
-    <t>Sincronizzazione  dell'orologio</t>
-  </si>
-  <si>
-    <t>Gli orologi dei sistemi di elaborazione delle  informazioni utilizzati dall'organizzazione devono  essere sincronizzati con fonti temporali approvate.</t>
-  </si>
-  <si>
-    <t>Utilizzo di programmi utility  privilegiati</t>
-  </si>
-  <si>
-    <t>L'uso di programmi utility che possono essere in grado  di aggirare i controlli di sistema e delle applicazioni  deve essere limitato e strettamente controllato.</t>
-  </si>
-  <si>
-    <t>Installazione di software sui  sistemi operativi</t>
-  </si>
-  <si>
-    <t>Procedure e misure devono essere implementate per  gestire in modo sicuro l'installazione di software sui  sistemi operativi.</t>
-  </si>
-  <si>
     <t>Sicurezza delle reti</t>
   </si>
   <si>
-    <t>Le reti e i dispositivi di rete devono essere protetti,  gestiti e controllati per proteggere le informazioni nei  sistemi.</t>
-  </si>
-  <si>
-    <t>Sicurezza dei servizi di rete  Controllo</t>
-  </si>
-  <si>
-    <t>I meccanismi di sicurezza, i livelli di servizio e i requisiti  di servizio dei servizi di rete devono essere identificati,  implementati e monitorati.</t>
-  </si>
-  <si>
     <t>Segregazione delle reti</t>
   </si>
   <si>
-    <t>Gruppi di servizi informativi, utenti e sistemi informativi  devono essere segregati nelle reti dell'organizzazione.</t>
-  </si>
-  <si>
     <t>Filtraggio web</t>
   </si>
   <si>
-    <t>L'accesso ai siti web esterni deve essere gestito per  ridurre l'esposizione a contenuti dannosi.</t>
-  </si>
-  <si>
     <t>Utilizzo della crittografia</t>
   </si>
   <si>
-    <t>Devono essere definite e implementate regole per  l'efficace utilizzo della crittografia, inclusa la gestione  delle chiavi crittografiche.</t>
-  </si>
-  <si>
-    <t>Ciclo di vita dello sviluppo  sicuro</t>
-  </si>
-  <si>
-    <t>Devono essere stabiliti e applicati principi per lo  sviluppo sicuro di software e sistemi.</t>
-  </si>
-  <si>
-    <t>Requisiti di sicurezza delle  applicazioni</t>
-  </si>
-  <si>
-    <t>I requisiti di sicurezza delle informazioni devono essere  identificati, specificati e approvati durante lo sviluppo o  l'acquisizione di applicazioni.</t>
-  </si>
-  <si>
-    <t>Architettura di sistema  sicuro e principi di  ingegneria</t>
-  </si>
-  <si>
-    <t>Devono essere stabiliti, documentati, mantenuti e  applicati principi per l'ingegneria di sistemi sicuri a tutte  le attività di sviluppo di sistemi informativi.</t>
-  </si>
-  <si>
     <t>Codifica sicura</t>
   </si>
   <si>
-    <t>Principi di codifica sicura devono essere applicati allo  sviluppo del software.</t>
-  </si>
-  <si>
-    <t>Test di sicurezza nello  sviluppo e nell'accettazione</t>
-  </si>
-  <si>
-    <t>I processi di test di sicurezza devono essere definiti e  implementati nel ciclo di vita dello sviluppo.</t>
-  </si>
-  <si>
     <t>Sviluppo esterno</t>
   </si>
   <si>
-    <t>L'organizzazione deve dirigere, monitorare e rivedere le  attività relative allo sviluppo esterno dei sistemi.</t>
-  </si>
-  <si>
-    <t>Separazione degli ambienti  di sviluppo, test e  produzione</t>
-  </si>
-  <si>
-    <t>Gli ambienti di sviluppo, test e produzione devono  essere separati e protetti.</t>
-  </si>
-  <si>
     <t>Gestione dei cambiamenti</t>
   </si>
   <si>
-    <t>I cambiamenti alle strutture di elaborazione delle  informazioni e ai sistemi informativi devono essere  soggetti a procedure di gestione dei cambiamenti.</t>
-  </si>
-  <si>
     <t>Informazioni di test</t>
   </si>
   <si>
-    <t>Le informazioni di test devono essere selezionate,  protette e gestite in modo appropriato.</t>
-  </si>
-  <si>
-    <t>Protezione dei sistemi  informativi durante i test di  audit</t>
-  </si>
-  <si>
-    <t>I test di audit e altre attività di garanzia che coinvolgono  la valutazione dei sistemi operativi devono essere  pianificati e concordati tra il tester e la gestione  appropriata.</t>
-  </si>
-  <si>
     <t>name[it]</t>
   </si>
   <si>
@@ -5681,6 +5234,453 @@
   </si>
   <si>
     <t>Questo schema riferisce lo standard ISO27001-2022.Puoi acquistarne una copia qui https://www.iso.org/standard/27001</t>
+  </si>
+  <si>
+    <t>Politiche per la sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>La politica di sicurezza delle informazioni e le politiche specifiche per argomento devono essere definite, approvate dalla direzione, pubblicate, comunicate e riconosciute dal personale rilevante e dalle parti interessate pertinenti, e revisionate a intervalli pianificati e in caso di cambiamenti significativi.</t>
+  </si>
+  <si>
+    <t>Ruoli e responsabilità per la sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>I ruoli e le responsabilità per la sicurezza delle informazioni devono essere definiti e assegnati in base alle esigenze dell'organizzazione.</t>
+  </si>
+  <si>
+    <t>I compiti in conflitto e le aree di responsabilità in conflitto devono essere separate.</t>
+  </si>
+  <si>
+    <t>Responsabilità della direzione</t>
+  </si>
+  <si>
+    <t>La direzione deve richiedere a tutto il personale di applicare la sicurezza delle informazioni in conformità con la politica di sicurezza delle informazioni stabilita, le politiche specifiche per argomento e le procedure dell'organizzazione.</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve stabilire e mantenere contatti con le autorità pertinenti.</t>
+  </si>
+  <si>
+    <t>Contatti con gruppi di interesse speciale</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve stabilire e mantenere contatti con gruppi di interesse speciale o altri forum specialistici sulla sicurezza e associazioni professionali.</t>
+  </si>
+  <si>
+    <t>Le informazioni relative alle minacce alla sicurezza delle informazioni devono essere raccolte e analizzate per produrre intelligence sulle minacce.</t>
+  </si>
+  <si>
+    <t>Sicurezza delle informazioni nella gestione dei progetti</t>
+  </si>
+  <si>
+    <t>La sicurezza delle informazioni deve essere integrata nella gestione dei progetti.</t>
+  </si>
+  <si>
+    <t>Inventario delle informazioni e di altri asset associati</t>
+  </si>
+  <si>
+    <t>Deve essere sviluppato e mantenuto un inventario delle informazioni e degli altri asset associati, inclusi i proprietari.</t>
+  </si>
+  <si>
+    <t>Utilizzo accettabile delle informazioni e di altri asset associati</t>
+  </si>
+  <si>
+    <t>Devono essere identificate, documentate e implementate regole per l'utilizzo accettabile e procedure per la gestione delle informazioni e degli altri asset associati.</t>
+  </si>
+  <si>
+    <t>Il personale e altre parti interessate, se appropriato, devono restituire tutti gli asset dell'organizzazione in loro possesso al momento del cambiamento o della cessazione del loro impiego, contratto o accordo.</t>
+  </si>
+  <si>
+    <t>Classificazione delle informazioni</t>
+  </si>
+  <si>
+    <t>Le informazioni devono essere classificate in base alle esigenze di sicurezza delle informazioni dell'organizzazione, in base a confidenzialità, integrità, disponibilità e requisiti pertinenti delle parti interessate.</t>
+  </si>
+  <si>
+    <t>Etichettatura delle informazioni</t>
+  </si>
+  <si>
+    <t>Deve essere sviluppato e implementato un insieme appropriato di procedure per l'etichettatura delle informazioni, in conformità con lo schema di classificazione delle informazioni adottato dall'organizzazione.</t>
+  </si>
+  <si>
+    <t>Trasferimento delle informazioni</t>
+  </si>
+  <si>
+    <t>Devono essere in vigore un insieme di regole, procedure o accordi per il trasferimento delle informazioni in tutti i tipi di strutture di trasferimento all'interno dell'organizzazione e tra l'organizzazione e altre parti.</t>
+  </si>
+  <si>
+    <t>Devono essere stabilite e implementate regole per controllare l'accesso fisico e logico alle informazioni e ad altri asset associati, in base ai requisiti aziendali e di sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Il ciclo di vita completo delle identità deve essere gestito.</t>
+  </si>
+  <si>
+    <t>Informazioni di autenticazione</t>
+  </si>
+  <si>
+    <t>L'assegnazione e la gestione delle informazioni di autenticazione devono essere controllate da un processo gestionale, incluso l'avviso al personale sull'adeguato trattamento delle informazioni di autenticazione.</t>
+  </si>
+  <si>
+    <t>I diritti di accesso alle informazioni e ad altri asset associati devono essere forniti, revisionati, modificati e rimossi in conformità con la politica specifica per argomento e le regole dell'organizzazione per il controllo degli accessi.</t>
+  </si>
+  <si>
+    <t>Sicurezza delle informazioni nelle relazioni con i fornitori</t>
+  </si>
+  <si>
+    <t>Devono essere definite e implementate procedure e processi per gestire i rischi per la sicurezza delle informazioni associati all'uso dei prodotti o servizi del fornitore.</t>
+  </si>
+  <si>
+    <t>Affrontare la sicurezza delle informazioni nei contratti con i fornitori</t>
+  </si>
+  <si>
+    <t>Requisiti pertinenti per la sicurezza delle informazioni devono essere stabiliti e concordati con ciascun fornitore in base al tipo di relazione con il fornitore.</t>
+  </si>
+  <si>
+    <t>Gestione della sicurezza delle informazioni nella catena di approvvigionamento ICT</t>
+  </si>
+  <si>
+    <t>Devono essere definiti e implementati processi e procedure per gestire i rischi per la sicurezza delle informazioni associati alla catena di approvvigionamento di prodotti e servizi ICT.</t>
+  </si>
+  <si>
+    <t>Monitoraggio, revisione e gestione dei servizi dei fornitori</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve monitorare regolarmente, revisionare, valutare e gestire i cambiamenti nelle pratiche di sicurezza delle informazioni e nella fornitura dei servizi da parte dei fornitori.</t>
+  </si>
+  <si>
+    <t>Sicurezza delle informazioni per l'uso dei servizi cloud</t>
+  </si>
+  <si>
+    <t>Devono essere stabiliti processi per l'acquisizione, l'uso, la gestione e l'uscita dai servizi cloud in conformità con i requisiti di sicurezza delle informazioni dell'organizzazione.</t>
+  </si>
+  <si>
+    <t>Pianificazione e preparazione per la gestione degli incidenti di sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve pianificare e prepararsi per gestire gli incidenti di sicurezza delle informazioni definendo, istituendo e comunicando processi, ruoli e responsabilità per la gestione degli incidenti di sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Valutazione e decisione sugli eventi di sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve valutare gli eventi di sicurezza delle informazioni e decidere se devono essere categorizzati come incidenti di sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Risposta agli incidenti di sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>Gli incidenti di sicurezza delle informazioni devono essere gestiti in conformità con le procedure documentate.</t>
+  </si>
+  <si>
+    <t>Apprendimento dagli incidenti di sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>Le conoscenze acquisite dagli incidenti di sicurezza delle informazioni devono essere utilizzate per rafforzare e migliorare i controlli della sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve stabilire e implementare procedure per l'identificazione, la raccolta, l'acquisizione e la conservazione di prove relative agli eventi di sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Sicurezza delle informazioni durante la distruzione</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve pianificare come mantenere la sicurezza delle informazioni ad un livello appropriato durante la distruzione.</t>
+  </si>
+  <si>
+    <t>Prontezza ICT per la continuità aziendale</t>
+  </si>
+  <si>
+    <t>La prontezza ICT deve essere pianificata, implementata, mantenuta e testata in base agli obiettivi di continuità aziendale e ai requisiti di continuità ICT.</t>
+  </si>
+  <si>
+    <t>Requisiti legali, statutari, regolamentari e contrattuali</t>
+  </si>
+  <si>
+    <t>I requisiti legali, statutari, regolamentari e contrattuali rilevanti per la sicurezza delle informazioni devono essere identificati, documentati e mantenuti aggiornati.</t>
+  </si>
+  <si>
+    <t>Diritti di proprietà intellettuale</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve implementare procedure appropriate per proteggere i diritti di proprietà intellettuale.</t>
+  </si>
+  <si>
+    <t>I documenti devono essere protetti da perdita, distruzione, falsificazione, accesso non autorizzato e divulgazione non autorizzata.</t>
+  </si>
+  <si>
+    <t>Privacy e protezione delle informazioni personali identificabili (PII)</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve identificare e soddisfare i requisiti relativi alla tutela della privacy e alla protezione delle PII in conformità alle leggi, ai regolamenti applicabili e ai requisiti contrattuali.</t>
+  </si>
+  <si>
+    <t>Revisione indipendente della sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>L'approccio dell'organizzazione alla gestione della sicurezza delle informazioni e la sua implementazione, compresi persone, processi e tecnologie, devono essere periodicamente riesaminati in modo indipendente a intervalli pianificati o in caso di cambiamenti significativi.</t>
+  </si>
+  <si>
+    <t>Conformità alle politiche, regole e standard per la sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>La conformità alla politica di sicurezza delle informazioni dell'organizzazione, alle politiche specifiche per argomento, alle regole e agli standard deve essere regolarmente riesaminata.</t>
+  </si>
+  <si>
+    <t>Procedure operative documentate</t>
+  </si>
+  <si>
+    <t>Le procedure operative per le strutture di elaborazione delle informazioni devono essere documentate e messe a disposizione del personale che ne ha bisogno.</t>
+  </si>
+  <si>
+    <t>Verifiche di verifica del background su tutti i candidati per diventare personale devono essere effettuate prima di entrare a far parte dell'organizzazione e in modo continuativo, prendendo in considerazione le leggi, i regolamenti, l'etica applicabile e proporzionalmente alle esigenze aziendali, alla classificazione delle informazioni da accedere e ai rischi percepiti.</t>
+  </si>
+  <si>
+    <t>Termini e condizioni di impiego</t>
+  </si>
+  <si>
+    <t>I contratti di lavoro devono specificare le responsabilità del personale e dell'organizzazione per la sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Consapevolezza, formazione ed educazione sulla sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>Il personale dell'organizzazione e le parti interessate pertinenti devono ricevere adeguate consapevolezza, formazione ed educazione sulla sicurezza delle informazioni e aggiornamenti regolari della politica di sicurezza delle informazioni dell'organizzazione, delle politiche specifiche per argomento e delle procedure, in relazione alle loro mansioni.</t>
+  </si>
+  <si>
+    <t>Un processo disciplinare deve essere formalizzato e comunicato per intraprendere azioni contro il personale e altre parti interessate pertinenti che hanno commesso una violazione della politica di sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Responsabilità dopo la cessazione o il cambio di impiego</t>
+  </si>
+  <si>
+    <t>Le responsabilità e i doveri relativi alla sicurezza delle informazioni che rimangono validi dopo la cessazione o il cambio di impiego devono essere definiti, attuati e comunicati al personale e alle altre parti interessate pertinenti.</t>
+  </si>
+  <si>
+    <t>Accordi di riservatezza o non divulgazione</t>
+  </si>
+  <si>
+    <t>Gli accordi di riservatezza o non divulgazione che riflettono le esigenze dell'organizzazione per la protezione delle informazioni devono essere identificati, documentati, regolarmente riesaminati e firmati dal personale e dalle altre parti interessate pertinenti.</t>
+  </si>
+  <si>
+    <t>Devono essere implementate misure di sicurezza quando il personale lavora in remoto per proteggere le informazioni a cui si accede, elabora o memorizza al di fuori dei locali dell'organizzazione.</t>
+  </si>
+  <si>
+    <t>Segnalazione degli eventi relativi alla sicurezza delle informazioni</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve fornire un meccanismo affinché il personale possa segnalare in modo tempestivo eventi di sicurezza delle informazioni osservati o sospettati attraverso canali appropriati.</t>
+  </si>
+  <si>
+    <t>I perimetri di sicurezza devono essere definiti e utilizzati per proteggere aree che contengono informazioni e altri asset associati.</t>
+  </si>
+  <si>
+    <t>Le aree sicure devono essere protette da controlli di accesso appropriati e punti di accesso.</t>
+  </si>
+  <si>
+    <t>Sicurezza degli uffici, delle stanze e delle strutture</t>
+  </si>
+  <si>
+    <t>La sicurezza fisica degli uffici, delle stanze e delle strutture deve essere progettata e implementata.</t>
+  </si>
+  <si>
+    <t>Monitoraggio della sicurezza fisica</t>
+  </si>
+  <si>
+    <t>I locali devono essere monitorati continuamente per l'accesso fisico non autorizzato.</t>
+  </si>
+  <si>
+    <t>Protezione contro minacce fisiche e ambientali</t>
+  </si>
+  <si>
+    <t>La protezione contro minacce fisiche ed ambientali, come disastri naturali o altre minacce fisiche intenzionali o non intenzionali all'infrastruttura, deve essere progettata ed implementata.</t>
+  </si>
+  <si>
+    <t>Misure di sicurezza per lavorare in aree sicure devono essere progettate ed implementate.</t>
+  </si>
+  <si>
+    <t>Area di lavoro e schermo puliti</t>
+  </si>
+  <si>
+    <t>Norme per la pulizia della scrivania per documenti e supporti rimovibili e regole per lo schermo dei sistemi di elaborazione delle informazioni devono essere definite e applicate in modo appropriato.</t>
+  </si>
+  <si>
+    <t>Posizionamento e protezione dell'attrezzatura</t>
+  </si>
+  <si>
+    <t>L'attrezzatura deve essere posizionata in modo sicuro e protetta.</t>
+  </si>
+  <si>
+    <t>I supporti di memorizzazione devono essere gestiti durante il loro ciclo di vita di acquisizione, utilizzo, trasporto e smaltimento in conformità con lo schema di classificazione e i requisiti di gestione dell'organizzazione.</t>
+  </si>
+  <si>
+    <t>Le strutture di elaborazione delle informazioni devono essere protette da interruzioni di corrente e da altre interruzioni causate da malfunzionamenti nei servizi di supporto.</t>
+  </si>
+  <si>
+    <t>I cavi che trasportano alimentazione, dati o servizi di informazione di supporto devono essere protetti da intercettazioni, interferenze o danneggiamenti.</t>
+  </si>
+  <si>
+    <t>Manutenzione dell'attrezzatura</t>
+  </si>
+  <si>
+    <t>L'attrezzatura deve essere mantenuta correttamente per garantire la disponibilità, l'integrità e la riservatezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Smaltimento sicuro o riutilizzo dell'attrezzatura</t>
+  </si>
+  <si>
+    <t>Gli elementi di attrezzatura contenenti supporti di memorizzazione devono essere verificati per garantire che tutti i dati sensibili e i software con licenza siano stati rimossi o sovrascritti in modo sicuro prima dello smaltimento o riutilizzo.</t>
+  </si>
+  <si>
+    <t>Dispositivi terminali dell'utente</t>
+  </si>
+  <si>
+    <t>Le informazioni memorizzate su, elaborate da o accessibili tramite dispositivi terminali dell'utente devono essere protette.</t>
+  </si>
+  <si>
+    <t>L'assegnazione e l'uso dei diritti di accesso privilegiati devono essere limitati e gestiti.</t>
+  </si>
+  <si>
+    <t>Restrizione dell'accesso alle informazioni</t>
+  </si>
+  <si>
+    <t>L'accesso alle informazioni e ad altri asset associati deve essere limitato in conformità con la politica specifica per argomento sul controllo degli accessi.</t>
+  </si>
+  <si>
+    <t>L'accesso in lettura e scrittura al codice sorgente, agli strumenti di sviluppo e alle librerie software deve essere gestito in modo appropriato.</t>
+  </si>
+  <si>
+    <t>Tecnologie e procedure di autenticazione sicura devono essere implementate in base alle restrizioni di accesso alle informazioni e alla politica specifica per argomento sul controllo degli accessi.</t>
+  </si>
+  <si>
+    <t>L'uso delle risorse deve essere monitorato e adattato in linea con i requisiti di capacità attuali e previsti.</t>
+  </si>
+  <si>
+    <t>La protezione contro malware deve essere implementata e supportata da un'adeguata consapevolezza degli utenti.</t>
+  </si>
+  <si>
+    <t>Gestione delle vulnerabilità tecniche</t>
+  </si>
+  <si>
+    <t>Deve essere ottenuta informazione sulle vulnerabilità tecniche dei sistemi informativi in uso, valutata l'esposizione dell'organizzazione a tali vulnerabilità e adottate misure appropriate.</t>
+  </si>
+  <si>
+    <t>Gestione della configurazione</t>
+  </si>
+  <si>
+    <t>Le configurazioni, inclusa la configurazione della sicurezza, dell'hardware, del software, dei servizi e delle reti, devono essere stabilite, documentate, implementate, monitorate e revisionate.</t>
+  </si>
+  <si>
+    <t>Eliminazione delle informazioni</t>
+  </si>
+  <si>
+    <t>Le informazioni memorizzate nei sistemi informativi, nei dispositivi o in qualsiasi altro supporto di memorizzazione devono essere eliminate quando non sono più necessarie.</t>
+  </si>
+  <si>
+    <t>Il mascheramento dei dati deve essere utilizzato in conformità con la politica specifica per argomento sull'accesso e altre politiche specifiche correlate, e ai requisiti aziendali, considerando la legislazione applicabile.</t>
+  </si>
+  <si>
+    <t>Prevenzione della fuga di dati</t>
+  </si>
+  <si>
+    <t>Misure di prevenzione della fuga di dati devono essere applicate a sistemi, reti e ad altri dispositivi che elaborano, memorizzano o trasmettono informazioni sensibili.</t>
+  </si>
+  <si>
+    <t>Copie di backup di informazioni, software e sistemi devono essere mantenute e regolarmente testate in conformità con la politica specifica per argomento sul backup concordata.</t>
+  </si>
+  <si>
+    <t>Ridondanza delle strutture di elaborazione delle informazioni</t>
+  </si>
+  <si>
+    <t>Le strutture di elaborazione delle informazioni devono essere implementate con una ridondanza sufficiente per soddisfare i requisiti di disponibilità.</t>
+  </si>
+  <si>
+    <t>I registri che registrano attività, eccezioni, guasti e altri eventi rilevanti devono essere prodotti, memorizzati, protetti ed analizzati.</t>
+  </si>
+  <si>
+    <t>Reti, sistemi e applicazioni devono essere monitorati per comportamenti anomali e devono essere adottate azioni appropriate per valutare potenziali incidenti di sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>Sincronizzazione dell'orologio</t>
+  </si>
+  <si>
+    <t>Gli orologi dei sistemi di elaborazione delle informazioni utilizzati dall'organizzazione devono essere sincronizzati con fonti temporali approvate.</t>
+  </si>
+  <si>
+    <t>Utilizzo di programmi utility privilegiati</t>
+  </si>
+  <si>
+    <t>L'uso di programmi utility che possono essere in grado di aggirare i controlli di sistema e delle applicazioni deve essere limitato e strettamente controllato.</t>
+  </si>
+  <si>
+    <t>Installazione di software sui sistemi operativi</t>
+  </si>
+  <si>
+    <t>Procedure e misure devono essere implementate per gestire in modo sicuro l'installazione di software sui sistemi operativi.</t>
+  </si>
+  <si>
+    <t>Le reti e i dispositivi di rete devono essere protetti, gestiti e controllati per proteggere le informazioni nei sistemi.</t>
+  </si>
+  <si>
+    <t>Sicurezza dei servizi di rete Controllo</t>
+  </si>
+  <si>
+    <t>I meccanismi di sicurezza, i livelli di servizio e i requisiti di servizio dei servizi di rete devono essere identificati, implementati e monitorati.</t>
+  </si>
+  <si>
+    <t>Gruppi di servizi informativi, utenti e sistemi informativi devono essere segregati nelle reti dell'organizzazione.</t>
+  </si>
+  <si>
+    <t>L'accesso ai siti web esterni deve essere gestito per ridurre l'esposizione a contenuti dannosi.</t>
+  </si>
+  <si>
+    <t>Devono essere definite e implementate regole per l'efficace utilizzo della crittografia, inclusa la gestione delle chiavi crittografiche.</t>
+  </si>
+  <si>
+    <t>Ciclo di vita dello sviluppo sicuro</t>
+  </si>
+  <si>
+    <t>Devono essere stabiliti e applicati principi per lo sviluppo sicuro di software e sistemi.</t>
+  </si>
+  <si>
+    <t>Requisiti di sicurezza delle applicazioni</t>
+  </si>
+  <si>
+    <t>I requisiti di sicurezza delle informazioni devono essere identificati, specificati e approvati durante lo sviluppo o l'acquisizione di applicazioni.</t>
+  </si>
+  <si>
+    <t>Architettura di sistema sicuro e principi di ingegneria</t>
+  </si>
+  <si>
+    <t>Devono essere stabiliti, documentati, mantenuti e applicati principi per l'ingegneria di sistemi sicuri a tutte le attività di sviluppo di sistemi informativi.</t>
+  </si>
+  <si>
+    <t>Principi di codifica sicura devono essere applicati allo sviluppo del software.</t>
+  </si>
+  <si>
+    <t>Test di sicurezza nello sviluppo e nell'accettazione</t>
+  </si>
+  <si>
+    <t>I processi di test di sicurezza devono essere definiti e implementati nel ciclo di vita dello sviluppo.</t>
+  </si>
+  <si>
+    <t>L'organizzazione deve dirigere, monitorare e rivedere le attività relative allo sviluppo esterno dei sistemi.</t>
+  </si>
+  <si>
+    <t>Separazione degli ambienti di sviluppo, test e produzione</t>
+  </si>
+  <si>
+    <t>Gli ambienti di sviluppo, test e produzione devono essere separati e protetti.</t>
+  </si>
+  <si>
+    <t>I cambiamenti alle strutture di elaborazione delle informazioni e ai sistemi informativi devono essere soggetti a procedure di gestione dei cambiamenti.</t>
+  </si>
+  <si>
+    <t>Le informazioni di test devono essere selezionate, protette e gestite in modo appropriato.</t>
+  </si>
+  <si>
+    <t>Protezione dei sistemi informativi durante i test di audit</t>
+  </si>
+  <si>
+    <t>I test di audit e altre attività di garanzia che coinvolgono la valutazione dei sistemi operativi devono essere pianificati e concordati tra il tester e la gestione appropriata.</t>
   </si>
 </sst>
 </file>
@@ -6201,7 +6201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -6232,7 +6232,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1690</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -6397,26 +6397,26 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1802</v>
+        <v>1653</v>
       </c>
       <c r="B24" t="s">
-        <v>1804</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1803</v>
+        <v>1654</v>
       </c>
       <c r="B25" t="s">
-        <v>1805</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1876</v>
+        <v>1727</v>
       </c>
       <c r="B26" t="s">
-        <v>1877</v>
+        <v>1728</v>
       </c>
     </row>
   </sheetData>
@@ -6551,18 +6551,18 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1802</v>
+        <v>1653</v>
       </c>
       <c r="B15" t="s">
-        <v>1804</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1803</v>
+        <v>1654</v>
       </c>
       <c r="B16" t="s">
-        <v>1805</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -6582,8 +6582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q144"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="N135" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="Q141" sqref="Q141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6730,7 +6730,7 @@
         <v>1089</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>1806</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -6780,10 +6780,10 @@
         <v>1490</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>1807</v>
+        <v>1658</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>1842</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -6833,10 +6833,10 @@
         <v>1491</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>1808</v>
+        <v>1659</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>1843</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -6886,10 +6886,10 @@
         <v>1492</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>1809</v>
+        <v>1660</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>1844</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -6939,10 +6939,10 @@
         <v>1493</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>1810</v>
+        <v>1661</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>1845</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -7031,10 +7031,10 @@
         <v>1494</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>1811</v>
+        <v>1662</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>1846</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -7084,10 +7084,10 @@
         <v>1495</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>1812</v>
+        <v>1663</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>1847</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -7137,10 +7137,10 @@
         <v>1496</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>1813</v>
+        <v>1664</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>1848</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -7179,7 +7179,7 @@
         <v>1089</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>1814</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="48" x14ac:dyDescent="0.2">
@@ -7218,7 +7218,7 @@
         <v>1089</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>1815</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -7268,10 +7268,10 @@
         <v>1497</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>1816</v>
+        <v>1667</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>1849</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -7321,10 +7321,10 @@
         <v>1498</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>1817</v>
+        <v>1668</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>1850</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -7374,10 +7374,10 @@
         <v>1499</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>1818</v>
+        <v>1669</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>1851</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -7427,10 +7427,10 @@
         <v>1500</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>1819</v>
+        <v>1670</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>1852</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -7480,10 +7480,10 @@
         <v>1501</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>1820</v>
+        <v>1671</v>
       </c>
       <c r="Q18" s="8" t="s">
-        <v>1853</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -7522,7 +7522,7 @@
         <v>1089</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>1821</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -7572,10 +7572,10 @@
         <v>1502</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>1822</v>
+        <v>1673</v>
       </c>
       <c r="Q20" s="8" t="s">
-        <v>1854</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -7625,10 +7625,10 @@
         <v>1503</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>1823</v>
+        <v>1674</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>1855</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -7678,10 +7678,10 @@
         <v>1504</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>1824</v>
+        <v>1675</v>
       </c>
       <c r="Q22" s="8" t="s">
-        <v>1856</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -7731,10 +7731,10 @@
         <v>1505</v>
       </c>
       <c r="P23" s="8" t="s">
-        <v>1825</v>
+        <v>1676</v>
       </c>
       <c r="Q23" s="8" t="s">
-        <v>1857</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -7773,7 +7773,7 @@
         <v>1089</v>
       </c>
       <c r="P24" s="8" t="s">
-        <v>1826</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -7823,10 +7823,10 @@
         <v>1506</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>1816</v>
+        <v>1667</v>
       </c>
       <c r="Q25" s="8" t="s">
-        <v>1858</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -7876,10 +7876,10 @@
         <v>1507</v>
       </c>
       <c r="P26" s="8" t="s">
-        <v>1827</v>
+        <v>1678</v>
       </c>
       <c r="Q26" s="8" t="s">
-        <v>1859</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -7929,10 +7929,10 @@
         <v>1508</v>
       </c>
       <c r="P27" s="8" t="s">
-        <v>1828</v>
+        <v>1679</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>1860</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -7971,7 +7971,7 @@
         <v>1089</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>1829</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -8021,10 +8021,10 @@
         <v>1509</v>
       </c>
       <c r="P29" s="8" t="s">
-        <v>1830</v>
+        <v>1681</v>
       </c>
       <c r="Q29" s="8" t="s">
-        <v>1861</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -8074,10 +8074,10 @@
         <v>1510</v>
       </c>
       <c r="P30" s="8" t="s">
-        <v>1817</v>
+        <v>1668</v>
       </c>
       <c r="Q30" s="8" t="s">
-        <v>1862</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -8127,10 +8127,10 @@
         <v>1511</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>1818</v>
+        <v>1669</v>
       </c>
       <c r="Q31" s="8" t="s">
-        <v>1863</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -8169,7 +8169,7 @@
         <v>1089</v>
       </c>
       <c r="P32" s="8" t="s">
-        <v>1831</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -8219,10 +8219,10 @@
         <v>1512</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>1832</v>
+        <v>1683</v>
       </c>
       <c r="Q33" s="8" t="s">
-        <v>1864</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -8261,7 +8261,7 @@
         <v>1089</v>
       </c>
       <c r="P34" s="8" t="s">
-        <v>1833</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -8311,10 +8311,10 @@
         <v>1513</v>
       </c>
       <c r="P35" s="8" t="s">
-        <v>1816</v>
+        <v>1667</v>
       </c>
       <c r="Q35" s="8" t="s">
-        <v>1865</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -8364,10 +8364,10 @@
         <v>1514</v>
       </c>
       <c r="P36" s="8" t="s">
-        <v>1834</v>
+        <v>1685</v>
       </c>
       <c r="Q36" s="8" t="s">
-        <v>1866</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -8406,7 +8406,7 @@
         <v>1089</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>1835</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -8456,10 +8456,10 @@
         <v>1515</v>
       </c>
       <c r="P38" s="8" t="s">
-        <v>1816</v>
+        <v>1667</v>
       </c>
       <c r="Q38" s="8" t="s">
-        <v>1867</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -8509,10 +8509,10 @@
         <v>1516</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>1836</v>
+        <v>1687</v>
       </c>
       <c r="Q39" s="8" t="s">
-        <v>1868</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -8562,10 +8562,10 @@
         <v>1517</v>
       </c>
       <c r="P40" s="8" t="s">
-        <v>1837</v>
+        <v>1688</v>
       </c>
       <c r="Q40" s="8" t="s">
-        <v>1869</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -8604,7 +8604,7 @@
         <v>1089</v>
       </c>
       <c r="P41" s="8" t="s">
-        <v>1838</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -8654,10 +8654,10 @@
         <v>1518</v>
       </c>
       <c r="P42" s="8" t="s">
-        <v>1839</v>
+        <v>1690</v>
       </c>
       <c r="Q42" s="8" t="s">
-        <v>1870</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="102" x14ac:dyDescent="0.2">
@@ -8707,10 +8707,10 @@
         <v>1519</v>
       </c>
       <c r="P43" s="8" t="s">
-        <v>1840</v>
+        <v>1691</v>
       </c>
       <c r="Q43" s="8" t="s">
-        <v>1871</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -8746,7 +8746,7 @@
         <v>1089</v>
       </c>
       <c r="P44" s="8" t="s">
-        <v>1841</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -8782,7 +8782,7 @@
         <v>1089</v>
       </c>
       <c r="P45" s="8" t="s">
-        <v>1872</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="144" x14ac:dyDescent="0.2">
@@ -8832,10 +8832,10 @@
         <v>1520</v>
       </c>
       <c r="P46" s="8" t="s">
-        <v>1616</v>
+        <v>1729</v>
       </c>
       <c r="Q46" s="8" t="s">
-        <v>1617</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -8885,10 +8885,10 @@
         <v>1521</v>
       </c>
       <c r="P47" s="8" t="s">
-        <v>1618</v>
+        <v>1731</v>
       </c>
       <c r="Q47" s="8" t="s">
-        <v>1619</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -8938,10 +8938,10 @@
         <v>1522</v>
       </c>
       <c r="P48" s="8" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
       <c r="Q48" s="8" t="s">
-        <v>1621</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -8991,10 +8991,10 @@
         <v>1523</v>
       </c>
       <c r="P49" s="8" t="s">
-        <v>1622</v>
+        <v>1734</v>
       </c>
       <c r="Q49" s="8" t="s">
-        <v>1623</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -9044,10 +9044,10 @@
         <v>1524</v>
       </c>
       <c r="P50" s="8" t="s">
-        <v>1624</v>
+        <v>1617</v>
       </c>
       <c r="Q50" s="8" t="s">
-        <v>1625</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -9097,10 +9097,10 @@
         <v>1525</v>
       </c>
       <c r="P51" s="8" t="s">
-        <v>1626</v>
+        <v>1737</v>
       </c>
       <c r="Q51" s="8" t="s">
-        <v>1627</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -9150,10 +9150,10 @@
         <v>1526</v>
       </c>
       <c r="P52" s="8" t="s">
-        <v>1628</v>
+        <v>1618</v>
       </c>
       <c r="Q52" s="8" t="s">
-        <v>1629</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -9203,10 +9203,10 @@
         <v>1527</v>
       </c>
       <c r="P53" s="8" t="s">
-        <v>1630</v>
+        <v>1740</v>
       </c>
       <c r="Q53" s="8" t="s">
-        <v>1631</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -9256,10 +9256,10 @@
         <v>1528</v>
       </c>
       <c r="P54" s="8" t="s">
-        <v>1632</v>
+        <v>1742</v>
       </c>
       <c r="Q54" s="8" t="s">
-        <v>1633</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -9309,10 +9309,10 @@
         <v>1529</v>
       </c>
       <c r="P55" s="8" t="s">
-        <v>1634</v>
+        <v>1744</v>
       </c>
       <c r="Q55" s="8" t="s">
-        <v>1635</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -9362,10 +9362,10 @@
         <v>1530</v>
       </c>
       <c r="P56" s="8" t="s">
-        <v>1636</v>
+        <v>1619</v>
       </c>
       <c r="Q56" s="8" t="s">
-        <v>1637</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -9415,10 +9415,10 @@
         <v>1531</v>
       </c>
       <c r="P57" s="8" t="s">
-        <v>1638</v>
+        <v>1747</v>
       </c>
       <c r="Q57" s="8" t="s">
-        <v>1639</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -9468,10 +9468,10 @@
         <v>1532</v>
       </c>
       <c r="P58" s="8" t="s">
-        <v>1640</v>
+        <v>1749</v>
       </c>
       <c r="Q58" s="8" t="s">
-        <v>1641</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -9521,10 +9521,10 @@
         <v>1533</v>
       </c>
       <c r="P59" s="8" t="s">
-        <v>1642</v>
+        <v>1751</v>
       </c>
       <c r="Q59" s="8" t="s">
-        <v>1643</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -9574,10 +9574,10 @@
         <v>1534</v>
       </c>
       <c r="P60" s="8" t="s">
-        <v>1644</v>
+        <v>1620</v>
       </c>
       <c r="Q60" s="8" t="s">
-        <v>1645</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -9627,10 +9627,10 @@
         <v>1535</v>
       </c>
       <c r="P61" s="8" t="s">
-        <v>1646</v>
+        <v>1621</v>
       </c>
       <c r="Q61" s="8" t="s">
-        <v>1647</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -9680,10 +9680,10 @@
         <v>1536</v>
       </c>
       <c r="P62" s="8" t="s">
-        <v>1648</v>
+        <v>1755</v>
       </c>
       <c r="Q62" s="8" t="s">
-        <v>1649</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -9733,10 +9733,10 @@
         <v>1537</v>
       </c>
       <c r="P63" s="8" t="s">
-        <v>1650</v>
+        <v>1622</v>
       </c>
       <c r="Q63" s="8" t="s">
-        <v>1651</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -9786,10 +9786,10 @@
         <v>1538</v>
       </c>
       <c r="P64" s="8" t="s">
-        <v>1652</v>
+        <v>1758</v>
       </c>
       <c r="Q64" s="8" t="s">
-        <v>1653</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -9839,10 +9839,10 @@
         <v>1539</v>
       </c>
       <c r="P65" s="8" t="s">
-        <v>1654</v>
+        <v>1760</v>
       </c>
       <c r="Q65" s="8" t="s">
-        <v>1655</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -9892,10 +9892,10 @@
         <v>1540</v>
       </c>
       <c r="P66" s="8" t="s">
-        <v>1656</v>
+        <v>1762</v>
       </c>
       <c r="Q66" s="8" t="s">
-        <v>1657</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -9945,10 +9945,10 @@
         <v>1541</v>
       </c>
       <c r="P67" s="8" t="s">
-        <v>1658</v>
+        <v>1764</v>
       </c>
       <c r="Q67" s="8" t="s">
-        <v>1659</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -9998,10 +9998,10 @@
         <v>1542</v>
       </c>
       <c r="P68" s="8" t="s">
-        <v>1660</v>
+        <v>1766</v>
       </c>
       <c r="Q68" s="8" t="s">
-        <v>1661</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -10051,10 +10051,10 @@
         <v>1543</v>
       </c>
       <c r="P69" s="8" t="s">
-        <v>1662</v>
+        <v>1768</v>
       </c>
       <c r="Q69" s="8" t="s">
-        <v>1663</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -10104,10 +10104,10 @@
         <v>1544</v>
       </c>
       <c r="P70" s="8" t="s">
-        <v>1664</v>
+        <v>1770</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>1665</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -10157,10 +10157,10 @@
         <v>1545</v>
       </c>
       <c r="P71" s="8" t="s">
-        <v>1666</v>
+        <v>1772</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>1667</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -10210,10 +10210,10 @@
         <v>1546</v>
       </c>
       <c r="P72" s="8" t="s">
-        <v>1668</v>
+        <v>1774</v>
       </c>
       <c r="Q72" s="8" t="s">
-        <v>1669</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="73" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -10263,10 +10263,10 @@
         <v>1547</v>
       </c>
       <c r="P73" s="8" t="s">
-        <v>1670</v>
+        <v>1623</v>
       </c>
       <c r="Q73" s="8" t="s">
-        <v>1671</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -10316,10 +10316,10 @@
         <v>1548</v>
       </c>
       <c r="P74" s="8" t="s">
-        <v>1672</v>
+        <v>1777</v>
       </c>
       <c r="Q74" s="8" t="s">
-        <v>1673</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -10369,10 +10369,10 @@
         <v>1549</v>
       </c>
       <c r="P75" s="8" t="s">
-        <v>1674</v>
+        <v>1779</v>
       </c>
       <c r="Q75" s="8" t="s">
-        <v>1675</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -10422,10 +10422,10 @@
         <v>1550</v>
       </c>
       <c r="P76" s="8" t="s">
-        <v>1676</v>
+        <v>1781</v>
       </c>
       <c r="Q76" s="8" t="s">
-        <v>1677</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="77" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -10475,10 +10475,10 @@
         <v>1551</v>
       </c>
       <c r="P77" s="8" t="s">
-        <v>1678</v>
+        <v>1783</v>
       </c>
       <c r="Q77" s="8" t="s">
-        <v>1679</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="78" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -10528,10 +10528,10 @@
         <v>1552</v>
       </c>
       <c r="P78" s="8" t="s">
-        <v>1680</v>
+        <v>1624</v>
       </c>
       <c r="Q78" s="8" t="s">
-        <v>1681</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="79" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -10581,10 +10581,10 @@
         <v>1553</v>
       </c>
       <c r="P79" s="8" t="s">
-        <v>1682</v>
+        <v>1786</v>
       </c>
       <c r="Q79" s="8" t="s">
-        <v>1683</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="128" x14ac:dyDescent="0.2">
@@ -10634,10 +10634,10 @@
         <v>1554</v>
       </c>
       <c r="P80" s="8" t="s">
-        <v>1684</v>
+        <v>1788</v>
       </c>
       <c r="Q80" s="8" t="s">
-        <v>1685</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -10687,10 +10687,10 @@
         <v>1555</v>
       </c>
       <c r="P81" s="8" t="s">
-        <v>1686</v>
+        <v>1790</v>
       </c>
       <c r="Q81" s="8" t="s">
-        <v>1687</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -10740,10 +10740,10 @@
         <v>1556</v>
       </c>
       <c r="P82" s="8" t="s">
-        <v>1688</v>
+        <v>1792</v>
       </c>
       <c r="Q82" s="8" t="s">
-        <v>1689</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -10781,7 +10781,7 @@
         <v>1089</v>
       </c>
       <c r="P83" s="8" t="s">
-        <v>1873</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="176" x14ac:dyDescent="0.2">
@@ -10834,7 +10834,7 @@
         <v>615</v>
       </c>
       <c r="Q84" s="8" t="s">
-        <v>1691</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -10884,10 +10884,10 @@
         <v>1558</v>
       </c>
       <c r="P85" s="8" t="s">
-        <v>1692</v>
+        <v>1795</v>
       </c>
       <c r="Q85" s="8" t="s">
-        <v>1693</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="176" x14ac:dyDescent="0.2">
@@ -10937,10 +10937,10 @@
         <v>1559</v>
       </c>
       <c r="P86" s="8" t="s">
-        <v>1694</v>
+        <v>1797</v>
       </c>
       <c r="Q86" s="8" t="s">
-        <v>1695</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -10990,10 +10990,10 @@
         <v>1560</v>
       </c>
       <c r="P87" s="8" t="s">
-        <v>1696</v>
+        <v>1626</v>
       </c>
       <c r="Q87" s="8" t="s">
-        <v>1697</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -11043,10 +11043,10 @@
         <v>1561</v>
       </c>
       <c r="P88" s="8" t="s">
-        <v>1698</v>
+        <v>1800</v>
       </c>
       <c r="Q88" s="8" t="s">
-        <v>1699</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="89" spans="1:17" ht="128" x14ac:dyDescent="0.2">
@@ -11096,10 +11096,10 @@
         <v>1562</v>
       </c>
       <c r="P89" s="8" t="s">
-        <v>1700</v>
+        <v>1802</v>
       </c>
       <c r="Q89" s="8" t="s">
-        <v>1701</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -11149,10 +11149,10 @@
         <v>1563</v>
       </c>
       <c r="P90" s="8" t="s">
-        <v>1702</v>
+        <v>1627</v>
       </c>
       <c r="Q90" s="8" t="s">
-        <v>1703</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -11202,10 +11202,10 @@
         <v>1564</v>
       </c>
       <c r="P91" s="8" t="s">
-        <v>1704</v>
+        <v>1805</v>
       </c>
       <c r="Q91" s="8" t="s">
-        <v>1705</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -11243,7 +11243,7 @@
         <v>1089</v>
       </c>
       <c r="P92" s="8" t="s">
-        <v>1874</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -11293,10 +11293,10 @@
         <v>1565</v>
       </c>
       <c r="P93" s="8" t="s">
-        <v>1706</v>
+        <v>1628</v>
       </c>
       <c r="Q93" s="8" t="s">
-        <v>1707</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -11346,10 +11346,10 @@
         <v>1566</v>
       </c>
       <c r="P94" s="8" t="s">
-        <v>1708</v>
+        <v>1629</v>
       </c>
       <c r="Q94" s="8" t="s">
-        <v>1709</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -11399,10 +11399,10 @@
         <v>1567</v>
       </c>
       <c r="P95" s="8" t="s">
-        <v>1710</v>
+        <v>1809</v>
       </c>
       <c r="Q95" s="8" t="s">
-        <v>1711</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -11452,10 +11452,10 @@
         <v>1568</v>
       </c>
       <c r="P96" s="8" t="s">
-        <v>1712</v>
+        <v>1811</v>
       </c>
       <c r="Q96" s="8" t="s">
-        <v>1713</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="97" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -11505,10 +11505,10 @@
         <v>1569</v>
       </c>
       <c r="P97" s="8" t="s">
-        <v>1714</v>
+        <v>1813</v>
       </c>
       <c r="Q97" s="8" t="s">
-        <v>1715</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="98" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -11558,10 +11558,10 @@
         <v>1570</v>
       </c>
       <c r="P98" s="8" t="s">
-        <v>1716</v>
+        <v>1630</v>
       </c>
       <c r="Q98" s="8" t="s">
-        <v>1717</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="99" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -11611,10 +11611,10 @@
         <v>1571</v>
       </c>
       <c r="P99" s="8" t="s">
-        <v>1718</v>
+        <v>1816</v>
       </c>
       <c r="Q99" s="8" t="s">
-        <v>1719</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="100" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -11664,10 +11664,10 @@
         <v>1572</v>
       </c>
       <c r="P100" s="8" t="s">
-        <v>1720</v>
+        <v>1818</v>
       </c>
       <c r="Q100" s="8" t="s">
-        <v>1721</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="101" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -11717,10 +11717,10 @@
         <v>1573</v>
       </c>
       <c r="P101" s="8" t="s">
-        <v>1722</v>
+        <v>1631</v>
       </c>
       <c r="Q101" s="8" t="s">
-        <v>1723</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="102" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -11770,10 +11770,10 @@
         <v>1574</v>
       </c>
       <c r="P102" s="8" t="s">
-        <v>1724</v>
+        <v>1633</v>
       </c>
       <c r="Q102" s="8" t="s">
-        <v>1725</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="103" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -11823,10 +11823,10 @@
         <v>1575</v>
       </c>
       <c r="P103" s="8" t="s">
-        <v>1726</v>
+        <v>1634</v>
       </c>
       <c r="Q103" s="8" t="s">
-        <v>1727</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -11876,10 +11876,10 @@
         <v>1576</v>
       </c>
       <c r="P104" s="8" t="s">
-        <v>1728</v>
+        <v>1635</v>
       </c>
       <c r="Q104" s="8" t="s">
-        <v>1729</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="105" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -11929,10 +11929,10 @@
         <v>1577</v>
       </c>
       <c r="P105" s="8" t="s">
-        <v>1730</v>
+        <v>1823</v>
       </c>
       <c r="Q105" s="8" t="s">
-        <v>1731</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="106" spans="1:17" ht="112" x14ac:dyDescent="0.2">
@@ -11982,10 +11982,10 @@
         <v>1578</v>
       </c>
       <c r="P106" s="8" t="s">
-        <v>1732</v>
+        <v>1825</v>
       </c>
       <c r="Q106" s="8" t="s">
-        <v>1733</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="107" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -12023,7 +12023,7 @@
         <v>1089</v>
       </c>
       <c r="P107" s="8" t="s">
-        <v>1875</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="108" spans="1:17" ht="85" x14ac:dyDescent="0.2">
@@ -12073,10 +12073,10 @@
         <v>1579</v>
       </c>
       <c r="P108" s="8" t="s">
-        <v>1734</v>
+        <v>1827</v>
       </c>
       <c r="Q108" s="8" t="s">
-        <v>1735</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="109" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -12126,10 +12126,10 @@
         <v>1580</v>
       </c>
       <c r="P109" s="8" t="s">
-        <v>1736</v>
+        <v>1636</v>
       </c>
       <c r="Q109" s="8" t="s">
-        <v>1737</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="110" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -12179,10 +12179,10 @@
         <v>1581</v>
       </c>
       <c r="P110" s="8" t="s">
-        <v>1738</v>
+        <v>1830</v>
       </c>
       <c r="Q110" s="8" t="s">
-        <v>1739</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="111" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -12232,10 +12232,10 @@
         <v>1582</v>
       </c>
       <c r="P111" s="8" t="s">
-        <v>1740</v>
+        <v>1637</v>
       </c>
       <c r="Q111" s="8" t="s">
-        <v>1741</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="112" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -12285,10 +12285,10 @@
         <v>1583</v>
       </c>
       <c r="P112" s="8" t="s">
-        <v>1742</v>
+        <v>1638</v>
       </c>
       <c r="Q112" s="8" t="s">
-        <v>1743</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="113" spans="1:17" ht="68" x14ac:dyDescent="0.2">
@@ -12338,10 +12338,10 @@
         <v>1584</v>
       </c>
       <c r="P113" s="8" t="s">
-        <v>1744</v>
+        <v>1639</v>
       </c>
       <c r="Q113" s="8" t="s">
-        <v>1745</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="114" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -12391,10 +12391,10 @@
         <v>1585</v>
       </c>
       <c r="P114" s="8" t="s">
-        <v>1746</v>
+        <v>1640</v>
       </c>
       <c r="Q114" s="8" t="s">
-        <v>1747</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="115" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -12444,10 +12444,10 @@
         <v>1586</v>
       </c>
       <c r="P115" s="8" t="s">
-        <v>1748</v>
+        <v>1836</v>
       </c>
       <c r="Q115" s="8" t="s">
-        <v>1749</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="116" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -12497,10 +12497,10 @@
         <v>1587</v>
       </c>
       <c r="P116" s="8" t="s">
-        <v>1750</v>
+        <v>1838</v>
       </c>
       <c r="Q116" s="8" t="s">
-        <v>1751</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="117" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -12550,10 +12550,10 @@
         <v>1588</v>
       </c>
       <c r="P117" s="8" t="s">
-        <v>1752</v>
+        <v>1840</v>
       </c>
       <c r="Q117" s="8" t="s">
-        <v>1753</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="118" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -12603,10 +12603,10 @@
         <v>1589</v>
       </c>
       <c r="P118" s="8" t="s">
-        <v>1754</v>
+        <v>1641</v>
       </c>
       <c r="Q118" s="8" t="s">
-        <v>1755</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="119" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -12656,10 +12656,10 @@
         <v>1590</v>
       </c>
       <c r="P119" s="8" t="s">
-        <v>1756</v>
+        <v>1843</v>
       </c>
       <c r="Q119" s="8" t="s">
-        <v>1757</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -12709,10 +12709,10 @@
         <v>1591</v>
       </c>
       <c r="P120" s="8" t="s">
-        <v>1758</v>
+        <v>1642</v>
       </c>
       <c r="Q120" s="8" t="s">
-        <v>1759</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="121" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -12762,10 +12762,10 @@
         <v>1592</v>
       </c>
       <c r="P121" s="8" t="s">
-        <v>1760</v>
+        <v>1846</v>
       </c>
       <c r="Q121" s="8" t="s">
-        <v>1761</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="122" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -12815,10 +12815,10 @@
         <v>1593</v>
       </c>
       <c r="P122" s="8" t="s">
-        <v>1762</v>
+        <v>1643</v>
       </c>
       <c r="Q122" s="8" t="s">
-        <v>1763</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="123" spans="1:17" ht="96" x14ac:dyDescent="0.2">
@@ -12868,10 +12868,10 @@
         <v>1594</v>
       </c>
       <c r="P123" s="8" t="s">
-        <v>1764</v>
+        <v>1644</v>
       </c>
       <c r="Q123" s="8" t="s">
-        <v>1765</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="124" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -12921,10 +12921,10 @@
         <v>1595</v>
       </c>
       <c r="P124" s="8" t="s">
-        <v>1766</v>
+        <v>1850</v>
       </c>
       <c r="Q124" s="8" t="s">
-        <v>1767</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="125" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -12974,10 +12974,10 @@
         <v>1596</v>
       </c>
       <c r="P125" s="8" t="s">
-        <v>1768</v>
+        <v>1852</v>
       </c>
       <c r="Q125" s="8" t="s">
-        <v>1769</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="126" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -13027,10 +13027,10 @@
         <v>1597</v>
       </c>
       <c r="P126" s="8" t="s">
-        <v>1770</v>
+        <v>1854</v>
       </c>
       <c r="Q126" s="8" t="s">
-        <v>1771</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="127" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -13080,10 +13080,10 @@
         <v>1598</v>
       </c>
       <c r="P127" s="8" t="s">
-        <v>1772</v>
+        <v>1645</v>
       </c>
       <c r="Q127" s="8" t="s">
-        <v>1773</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="128" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -13133,10 +13133,10 @@
         <v>1599</v>
       </c>
       <c r="P128" s="8" t="s">
-        <v>1774</v>
+        <v>1857</v>
       </c>
       <c r="Q128" s="8" t="s">
-        <v>1775</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="129" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -13186,10 +13186,10 @@
         <v>1600</v>
       </c>
       <c r="P129" s="8" t="s">
-        <v>1776</v>
+        <v>1646</v>
       </c>
       <c r="Q129" s="8" t="s">
-        <v>1777</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="130" spans="1:17" ht="48" x14ac:dyDescent="0.2">
@@ -13239,10 +13239,10 @@
         <v>1601</v>
       </c>
       <c r="P130" s="8" t="s">
-        <v>1778</v>
+        <v>1647</v>
       </c>
       <c r="Q130" s="8" t="s">
-        <v>1779</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="131" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -13292,10 +13292,10 @@
         <v>1602</v>
       </c>
       <c r="P131" s="8" t="s">
-        <v>1780</v>
+        <v>1648</v>
       </c>
       <c r="Q131" s="8" t="s">
-        <v>1781</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="132" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -13345,10 +13345,10 @@
         <v>1603</v>
       </c>
       <c r="P132" s="8" t="s">
-        <v>1782</v>
+        <v>1862</v>
       </c>
       <c r="Q132" s="8" t="s">
-        <v>1783</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="133" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -13398,10 +13398,10 @@
         <v>1604</v>
       </c>
       <c r="P133" s="8" t="s">
-        <v>1784</v>
+        <v>1864</v>
       </c>
       <c r="Q133" s="8" t="s">
-        <v>1785</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="134" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -13451,10 +13451,10 @@
         <v>1605</v>
       </c>
       <c r="P134" s="8" t="s">
-        <v>1786</v>
+        <v>1866</v>
       </c>
       <c r="Q134" s="8" t="s">
-        <v>1787</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="135" spans="1:17" ht="34" x14ac:dyDescent="0.2">
@@ -13504,10 +13504,10 @@
         <v>1606</v>
       </c>
       <c r="P135" s="8" t="s">
-        <v>1788</v>
+        <v>1649</v>
       </c>
       <c r="Q135" s="8" t="s">
-        <v>1789</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="136" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -13557,10 +13557,10 @@
         <v>1607</v>
       </c>
       <c r="P136" s="8" t="s">
-        <v>1790</v>
+        <v>1869</v>
       </c>
       <c r="Q136" s="8" t="s">
-        <v>1791</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="137" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -13610,10 +13610,10 @@
         <v>1608</v>
       </c>
       <c r="P137" s="8" t="s">
-        <v>1792</v>
+        <v>1650</v>
       </c>
       <c r="Q137" s="8" t="s">
-        <v>1793</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="138" spans="1:17" ht="64" x14ac:dyDescent="0.2">
@@ -13663,10 +13663,10 @@
         <v>1609</v>
       </c>
       <c r="P138" s="8" t="s">
-        <v>1794</v>
+        <v>1872</v>
       </c>
       <c r="Q138" s="8" t="s">
-        <v>1795</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="139" spans="1:17" ht="80" x14ac:dyDescent="0.2">
@@ -13716,10 +13716,10 @@
         <v>1610</v>
       </c>
       <c r="P139" s="8" t="s">
-        <v>1796</v>
+        <v>1651</v>
       </c>
       <c r="Q139" s="8" t="s">
-        <v>1797</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="140" spans="1:17" ht="48" x14ac:dyDescent="0.2">
@@ -13769,10 +13769,10 @@
         <v>1611</v>
       </c>
       <c r="P140" s="8" t="s">
-        <v>1798</v>
+        <v>1652</v>
       </c>
       <c r="Q140" s="8" t="s">
-        <v>1799</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="141" spans="1:17" ht="85" x14ac:dyDescent="0.2">
@@ -13822,10 +13822,10 @@
         <v>1612</v>
       </c>
       <c r="P141" s="8" t="s">
-        <v>1800</v>
+        <v>1876</v>
       </c>
       <c r="Q141" s="8" t="s">
-        <v>1801</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="142" spans="1:17" ht="16" x14ac:dyDescent="0.2">
@@ -13890,8 +13890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="K11" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13993,10 +13993,10 @@
         <v>1520</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>1616</v>
+        <v>1729</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>1617</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -14037,10 +14037,10 @@
         <v>1521</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>1618</v>
+        <v>1731</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>1619</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14081,10 +14081,10 @@
         <v>1522</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>1621</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -14125,10 +14125,10 @@
         <v>1523</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>1622</v>
+        <v>1734</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>1623</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -14169,10 +14169,10 @@
         <v>1524</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>1624</v>
+        <v>1617</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>1625</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14213,10 +14213,10 @@
         <v>1525</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>1626</v>
+        <v>1737</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>1627</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -14257,10 +14257,10 @@
         <v>1526</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>1628</v>
+        <v>1618</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>1629</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14301,10 +14301,10 @@
         <v>1527</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>1630</v>
+        <v>1740</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>1631</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14345,10 +14345,10 @@
         <v>1528</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>1632</v>
+        <v>1742</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>1633</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -14389,10 +14389,10 @@
         <v>1529</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>1634</v>
+        <v>1744</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>1635</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14433,10 +14433,10 @@
         <v>1530</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>1636</v>
+        <v>1619</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>1637</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -14477,10 +14477,10 @@
         <v>1531</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>1638</v>
+        <v>1747</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>1639</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14521,10 +14521,10 @@
         <v>1532</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>1640</v>
+        <v>1749</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>1641</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14565,10 +14565,10 @@
         <v>1533</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>1642</v>
+        <v>1751</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>1643</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14609,10 +14609,10 @@
         <v>1534</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>1644</v>
+        <v>1620</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>1645</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14653,10 +14653,10 @@
         <v>1535</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>1646</v>
+        <v>1621</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>1647</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14697,10 +14697,10 @@
         <v>1536</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>1648</v>
+        <v>1755</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>1649</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14741,10 +14741,10 @@
         <v>1537</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>1650</v>
+        <v>1622</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>1651</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14785,10 +14785,10 @@
         <v>1538</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>1652</v>
+        <v>1758</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>1653</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14829,10 +14829,10 @@
         <v>1539</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>1654</v>
+        <v>1760</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>1655</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -14873,10 +14873,10 @@
         <v>1540</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>1656</v>
+        <v>1762</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>1657</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14917,10 +14917,10 @@
         <v>1541</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>1658</v>
+        <v>1764</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>1659</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -14961,10 +14961,10 @@
         <v>1542</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>1660</v>
+        <v>1766</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>1661</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15005,10 +15005,10 @@
         <v>1543</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>1662</v>
+        <v>1768</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>1663</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15049,10 +15049,10 @@
         <v>1544</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>1664</v>
+        <v>1770</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>1665</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15093,10 +15093,10 @@
         <v>1545</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>1666</v>
+        <v>1772</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>1667</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15137,10 +15137,10 @@
         <v>1546</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>1668</v>
+        <v>1774</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>1669</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15181,10 +15181,10 @@
         <v>1547</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>1670</v>
+        <v>1623</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>1671</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15225,10 +15225,10 @@
         <v>1548</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>1672</v>
+        <v>1777</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>1673</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15269,10 +15269,10 @@
         <v>1549</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>1674</v>
+        <v>1779</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>1675</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15313,10 +15313,10 @@
         <v>1550</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>1676</v>
+        <v>1781</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>1677</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15357,10 +15357,10 @@
         <v>1551</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>1678</v>
+        <v>1783</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>1679</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15401,10 +15401,10 @@
         <v>1552</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>1680</v>
+        <v>1624</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>1681</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15445,10 +15445,10 @@
         <v>1553</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>1682</v>
+        <v>1786</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>1683</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="96" x14ac:dyDescent="0.2">
@@ -15489,10 +15489,10 @@
         <v>1554</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>1684</v>
+        <v>1788</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>1685</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15533,10 +15533,10 @@
         <v>1555</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>1686</v>
+        <v>1790</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>1687</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -15577,10 +15577,10 @@
         <v>1556</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>1688</v>
+        <v>1792</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>1689</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="112" x14ac:dyDescent="0.2">
@@ -15624,7 +15624,7 @@
         <v>615</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>1691</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15665,10 +15665,10 @@
         <v>1558</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>1692</v>
+        <v>1795</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>1693</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -15709,10 +15709,10 @@
         <v>1559</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>1694</v>
+        <v>1797</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>1695</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15753,10 +15753,10 @@
         <v>1560</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>1696</v>
+        <v>1626</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>1697</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -15797,10 +15797,10 @@
         <v>1561</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>1698</v>
+        <v>1800</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>1699</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15841,10 +15841,10 @@
         <v>1562</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>1700</v>
+        <v>1802</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>1701</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -15885,10 +15885,10 @@
         <v>1563</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>1702</v>
+        <v>1627</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>1703</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15929,10 +15929,10 @@
         <v>1564</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>1704</v>
+        <v>1805</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>1705</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -15973,10 +15973,10 @@
         <v>1565</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>1706</v>
+        <v>1628</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>1707</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16017,10 +16017,10 @@
         <v>1566</v>
       </c>
       <c r="M48" s="8" t="s">
-        <v>1708</v>
+        <v>1629</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>1709</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16061,10 +16061,10 @@
         <v>1567</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>1710</v>
+        <v>1809</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>1711</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -16105,10 +16105,10 @@
         <v>1568</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>1712</v>
+        <v>1811</v>
       </c>
       <c r="N50" s="8" t="s">
-        <v>1713</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16149,10 +16149,10 @@
         <v>1569</v>
       </c>
       <c r="M51" s="8" t="s">
-        <v>1714</v>
+        <v>1813</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>1715</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16193,10 +16193,10 @@
         <v>1570</v>
       </c>
       <c r="M52" s="8" t="s">
-        <v>1716</v>
+        <v>1630</v>
       </c>
       <c r="N52" s="8" t="s">
-        <v>1717</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -16237,10 +16237,10 @@
         <v>1571</v>
       </c>
       <c r="M53" s="8" t="s">
-        <v>1718</v>
+        <v>1816</v>
       </c>
       <c r="N53" s="8" t="s">
-        <v>1719</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -16281,10 +16281,10 @@
         <v>1572</v>
       </c>
       <c r="M54" s="8" t="s">
-        <v>1720</v>
+        <v>1818</v>
       </c>
       <c r="N54" s="8" t="s">
-        <v>1721</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16325,10 +16325,10 @@
         <v>1573</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>1722</v>
+        <v>1631</v>
       </c>
       <c r="N55" s="8" t="s">
-        <v>1723</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -16369,10 +16369,10 @@
         <v>1574</v>
       </c>
       <c r="M56" s="8" t="s">
-        <v>1724</v>
+        <v>1633</v>
       </c>
       <c r="N56" s="8" t="s">
-        <v>1725</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16413,10 +16413,10 @@
         <v>1575</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>1726</v>
+        <v>1634</v>
       </c>
       <c r="N57" s="8" t="s">
-        <v>1727</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16457,10 +16457,10 @@
         <v>1576</v>
       </c>
       <c r="M58" s="8" t="s">
-        <v>1728</v>
+        <v>1635</v>
       </c>
       <c r="N58" s="8" t="s">
-        <v>1729</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -16501,10 +16501,10 @@
         <v>1577</v>
       </c>
       <c r="M59" s="8" t="s">
-        <v>1730</v>
+        <v>1823</v>
       </c>
       <c r="N59" s="8" t="s">
-        <v>1731</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16545,10 +16545,10 @@
         <v>1578</v>
       </c>
       <c r="M60" s="8" t="s">
-        <v>1732</v>
+        <v>1825</v>
       </c>
       <c r="N60" s="8" t="s">
-        <v>1733</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -16589,10 +16589,10 @@
         <v>1579</v>
       </c>
       <c r="M61" s="8" t="s">
-        <v>1734</v>
+        <v>1827</v>
       </c>
       <c r="N61" s="8" t="s">
-        <v>1735</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -16633,10 +16633,10 @@
         <v>1580</v>
       </c>
       <c r="M62" s="8" t="s">
-        <v>1736</v>
+        <v>1636</v>
       </c>
       <c r="N62" s="8" t="s">
-        <v>1737</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -16677,10 +16677,10 @@
         <v>1581</v>
       </c>
       <c r="M63" s="8" t="s">
-        <v>1738</v>
+        <v>1830</v>
       </c>
       <c r="N63" s="8" t="s">
-        <v>1739</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16721,10 +16721,10 @@
         <v>1582</v>
       </c>
       <c r="M64" s="8" t="s">
-        <v>1740</v>
+        <v>1637</v>
       </c>
       <c r="N64" s="8" t="s">
-        <v>1741</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -16765,10 +16765,10 @@
         <v>1583</v>
       </c>
       <c r="M65" s="8" t="s">
-        <v>1742</v>
+        <v>1638</v>
       </c>
       <c r="N65" s="8" t="s">
-        <v>1743</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16809,10 +16809,10 @@
         <v>1584</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>1744</v>
+        <v>1639</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>1745</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16853,10 +16853,10 @@
         <v>1585</v>
       </c>
       <c r="M67" s="8" t="s">
-        <v>1746</v>
+        <v>1640</v>
       </c>
       <c r="N67" s="8" t="s">
-        <v>1747</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -16897,10 +16897,10 @@
         <v>1586</v>
       </c>
       <c r="M68" s="8" t="s">
-        <v>1748</v>
+        <v>1836</v>
       </c>
       <c r="N68" s="8" t="s">
-        <v>1749</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -16941,10 +16941,10 @@
         <v>1587</v>
       </c>
       <c r="M69" s="8" t="s">
-        <v>1750</v>
+        <v>1838</v>
       </c>
       <c r="N69" s="8" t="s">
-        <v>1751</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -16985,10 +16985,10 @@
         <v>1588</v>
       </c>
       <c r="M70" s="8" t="s">
-        <v>1752</v>
+        <v>1840</v>
       </c>
       <c r="N70" s="8" t="s">
-        <v>1753</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -17029,10 +17029,10 @@
         <v>1589</v>
       </c>
       <c r="M71" s="8" t="s">
-        <v>1754</v>
+        <v>1641</v>
       </c>
       <c r="N71" s="8" t="s">
-        <v>1755</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17073,10 +17073,10 @@
         <v>1590</v>
       </c>
       <c r="M72" s="8" t="s">
-        <v>1756</v>
+        <v>1843</v>
       </c>
       <c r="N72" s="8" t="s">
-        <v>1757</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17117,10 +17117,10 @@
         <v>1591</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>1758</v>
+        <v>1642</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>1759</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17161,10 +17161,10 @@
         <v>1592</v>
       </c>
       <c r="M74" s="8" t="s">
-        <v>1760</v>
+        <v>1846</v>
       </c>
       <c r="N74" s="8" t="s">
-        <v>1761</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17205,10 +17205,10 @@
         <v>1593</v>
       </c>
       <c r="M75" s="8" t="s">
-        <v>1762</v>
+        <v>1643</v>
       </c>
       <c r="N75" s="8" t="s">
-        <v>1763</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="64" x14ac:dyDescent="0.2">
@@ -17249,10 +17249,10 @@
         <v>1594</v>
       </c>
       <c r="M76" s="8" t="s">
-        <v>1764</v>
+        <v>1644</v>
       </c>
       <c r="N76" s="8" t="s">
-        <v>1765</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17293,10 +17293,10 @@
         <v>1595</v>
       </c>
       <c r="M77" s="8" t="s">
-        <v>1766</v>
+        <v>1850</v>
       </c>
       <c r="N77" s="8" t="s">
-        <v>1767</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -17337,10 +17337,10 @@
         <v>1596</v>
       </c>
       <c r="M78" s="8" t="s">
-        <v>1768</v>
+        <v>1852</v>
       </c>
       <c r="N78" s="8" t="s">
-        <v>1769</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17381,10 +17381,10 @@
         <v>1597</v>
       </c>
       <c r="M79" s="8" t="s">
-        <v>1770</v>
+        <v>1854</v>
       </c>
       <c r="N79" s="8" t="s">
-        <v>1771</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -17425,10 +17425,10 @@
         <v>1598</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>1772</v>
+        <v>1645</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>1773</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17469,10 +17469,10 @@
         <v>1599</v>
       </c>
       <c r="M81" s="8" t="s">
-        <v>1774</v>
+        <v>1857</v>
       </c>
       <c r="N81" s="8" t="s">
-        <v>1775</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17513,10 +17513,10 @@
         <v>1600</v>
       </c>
       <c r="M82" s="8" t="s">
-        <v>1776</v>
+        <v>1646</v>
       </c>
       <c r="N82" s="8" t="s">
-        <v>1777</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -17557,10 +17557,10 @@
         <v>1601</v>
       </c>
       <c r="M83" s="8" t="s">
-        <v>1778</v>
+        <v>1647</v>
       </c>
       <c r="N83" s="8" t="s">
-        <v>1779</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17601,10 +17601,10 @@
         <v>1602</v>
       </c>
       <c r="M84" s="8" t="s">
-        <v>1780</v>
+        <v>1648</v>
       </c>
       <c r="N84" s="8" t="s">
-        <v>1781</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17645,10 +17645,10 @@
         <v>1603</v>
       </c>
       <c r="M85" s="8" t="s">
-        <v>1782</v>
+        <v>1862</v>
       </c>
       <c r="N85" s="8" t="s">
-        <v>1783</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -17689,10 +17689,10 @@
         <v>1604</v>
       </c>
       <c r="M86" s="8" t="s">
-        <v>1784</v>
+        <v>1864</v>
       </c>
       <c r="N86" s="8" t="s">
-        <v>1785</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -17733,10 +17733,10 @@
         <v>1605</v>
       </c>
       <c r="M87" s="8" t="s">
-        <v>1786</v>
+        <v>1866</v>
       </c>
       <c r="N87" s="8" t="s">
-        <v>1787</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -17777,10 +17777,10 @@
         <v>1606</v>
       </c>
       <c r="M88" s="8" t="s">
-        <v>1788</v>
+        <v>1649</v>
       </c>
       <c r="N88" s="8" t="s">
-        <v>1789</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17821,10 +17821,10 @@
         <v>1607</v>
       </c>
       <c r="M89" s="8" t="s">
-        <v>1790</v>
+        <v>1869</v>
       </c>
       <c r="N89" s="8" t="s">
-        <v>1791</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17865,10 +17865,10 @@
         <v>1608</v>
       </c>
       <c r="M90" s="8" t="s">
-        <v>1792</v>
+        <v>1650</v>
       </c>
       <c r="N90" s="8" t="s">
-        <v>1793</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17909,10 +17909,10 @@
         <v>1609</v>
       </c>
       <c r="M91" s="8" t="s">
-        <v>1794</v>
+        <v>1872</v>
       </c>
       <c r="N91" s="8" t="s">
-        <v>1795</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -17953,10 +17953,10 @@
         <v>1610</v>
       </c>
       <c r="M92" s="8" t="s">
-        <v>1796</v>
+        <v>1651</v>
       </c>
       <c r="N92" s="8" t="s">
-        <v>1797</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -17997,10 +17997,10 @@
         <v>1611</v>
       </c>
       <c r="M93" s="8" t="s">
-        <v>1798</v>
+        <v>1652</v>
       </c>
       <c r="N93" s="8" t="s">
-        <v>1799</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -18041,10 +18041,10 @@
         <v>1612</v>
       </c>
       <c r="M94" s="8" t="s">
-        <v>1800</v>
+        <v>1876</v>
       </c>
       <c r="N94" s="8" t="s">
-        <v>1801</v>
+        <v>1877</v>
       </c>
     </row>
   </sheetData>
@@ -18173,7 +18173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>